<commit_message>
Updating flag format for senate challenge
</commit_message>
<xml_diff>
--- a/challenges/crypto/i-am-the-senate/solution/Solution.xlsx
+++ b/challenges/crypto/i-am-the-senate/solution/Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan Solomon\Documents\Software\github\charger-hack-2022\challenges\crypto\i-am-the-senate\solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E81952AB-CECD-4499-8A8D-E624140796CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6172B8C4-8439-46F6-A5D6-DED8F10E43A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2B46BE1-56B3-4226-8F38-A6268DEFB568}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>DiDiDDDDiidydydydyddououooouuoevevvvvevverererreerhehheehhhhararrrararthththhhhhetetetetetraraaraaargegeeggeggdyddyyddyyofofffoofoDaDaDaaaaartrrttrrtthPhPPPhhPPlalaaalallgugguugggueieiieiieisTssTTsTssheheeehehhWiWWiiWWiiseseseeeeeItIttIttIthohoooohhouguguggggghthtthhhthnonnoonnnotItIItIIIttsttsststtnonooonnontataaaattastststttttoroorroorrytyttytttyheheehhheeJeJeeeJJeJdidiiiiddiwowooowwwwulullluluudtddttdddteleelleeeelylyylyyylououuuuuou</t>
+    <t>DiDiDiDiDidydydddddyououoouoooevevvvvevverererreerhehheehhhhararrrararthththhhhhetetetetetraraaraaargegeeggeggdyddyyddyyofofffoofoDaDaDaaaaartrrttrrtthPhPPPhhPPlalaaalallgugguugggueieiieiieisTssTTsTssheheeehehhWiWWiiWWiiseseseeeeeItIttIttIthohoooohhouguguggggghthtthhhthnonnoonnnotItIItIIIttsttsststtnonooonnontataaaattastststttttoroorroorrytyttytttyheheehhheeJeJeeeJJeJdidiiiiddiwowooowwwwulullluluudtddttdddteleelleeeelylyylyyylououuuuuou</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:W213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
       </c>
       <c r="B3" t="str">
         <f>MID($B$1,A3,10)</f>
-        <v>DiDiDDDDii</v>
+        <v>DiDiDiDiDi</v>
       </c>
       <c r="C3" t="str">
         <f>MID($B3,C$2,1)</f>
@@ -464,7 +464,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
-        <v>D</v>
+        <v>i</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -472,11 +472,11 @@
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v>D</v>
+        <v>i</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
-        <v>i</v>
+        <v>D</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
@@ -496,7 +496,7 @@
       </c>
       <c r="P3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
@@ -504,11 +504,11 @@
       </c>
       <c r="R3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <f t="shared" si="1"/>
@@ -516,15 +516,15 @@
       </c>
       <c r="U3" t="str">
         <f>_xlfn.CONCAT(M3:T3)</f>
-        <v>01000011</v>
+        <v>01010101</v>
       </c>
       <c r="V3" t="str">
         <f>CHAR(BIN2DEC(U3))</f>
-        <v>C</v>
+        <v>U</v>
       </c>
       <c r="W3" t="str">
         <f>_xlfn.CONCAT(V3:V46)</f>
-        <v>CTF{Y0u_Und3r_3st1m4t3_my_b1n4ry_3ncrypt10n}</v>
+        <v>UAH{Y0u_Und3r_3st1m4t3_my_b1n4ry_3ncrypt10n}</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -533,10 +533,10 @@
       </c>
       <c r="B4" t="str">
         <f>MID($B$1,A4,10)</f>
-        <v>dydydydydd</v>
+        <v>dydydddddy</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:L67" si="2">MID($B4,C$2,1)</f>
+        <f t="shared" ref="C4:L42" si="2">MID($B4,C$2,1)</f>
         <v>d</v>
       </c>
       <c r="D4" t="str">
@@ -557,7 +557,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>y</v>
+        <v>d</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>y</v>
+        <v>d</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>d</v>
+        <v>y</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M67" si="3">IF(E4=$C4, 0, 1)</f>
@@ -589,7 +589,7 @@
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P67" si="6">IF(H4=$C4, 0, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
         <f t="shared" ref="Q4:Q67" si="7">IF(I4=$C4, 0, 1)</f>
@@ -597,7 +597,7 @@
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R67" si="8">IF(J4=$C4, 0, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <f t="shared" ref="S4:S67" si="9">IF(K4=$C4, 0, 1)</f>
@@ -605,15 +605,15 @@
       </c>
       <c r="T4">
         <f t="shared" ref="T4:T67" si="10">IF(L4=$C4, 0, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" t="str">
         <f t="shared" ref="U4:U67" si="11">_xlfn.CONCAT(M4:T4)</f>
-        <v>01010100</v>
+        <v>01000001</v>
       </c>
       <c r="V4" t="str">
         <f t="shared" ref="V4:V67" si="12">CHAR(BIN2DEC(U4))</f>
-        <v>T</v>
+        <v>A</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -622,7 +622,7 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" ref="B5:B68" si="13">MID($B$1,A5,10)</f>
-        <v>ououooouuo</v>
+        <v>ououoouooo</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="2"/>
@@ -650,15 +650,15 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>o</v>
+        <v>u</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>u</v>
+        <v>o</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
-        <v>u</v>
+        <v>o</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
@@ -682,15 +682,15 @@
       </c>
       <c r="Q5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <f t="shared" si="10"/>
@@ -698,11 +698,11 @@
       </c>
       <c r="U5" t="str">
         <f t="shared" si="11"/>
-        <v>01000110</v>
+        <v>01001000</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="12"/>
-        <v>F</v>
+        <v>H</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -4007,7 +4007,7 @@
         <v>dtddttdddt</v>
       </c>
       <c r="C43" t="str">
-        <f t="shared" ref="C43:L74" si="14">MID($B43,C$2,1)</f>
+        <f t="shared" ref="C43:L68" si="14">MID($B43,C$2,1)</f>
         <v>d</v>
       </c>
       <c r="D43" t="str">
@@ -6252,7 +6252,7 @@
         <v/>
       </c>
       <c r="H68" t="str">
-        <f t="shared" ref="D68:L131" si="15">MID($B68,H$2,1)</f>
+        <f t="shared" ref="D68:L96" si="15">MID($B68,H$2,1)</f>
         <v/>
       </c>
       <c r="I68" t="str">
@@ -8756,7 +8756,7 @@
         <v/>
       </c>
       <c r="K96" t="str">
-        <f t="shared" ref="D96:L159" si="28">MID($B96,K$2,1)</f>
+        <f t="shared" ref="D96:L125" si="28">MID($B96,K$2,1)</f>
         <v/>
       </c>
       <c r="L96" t="str">
@@ -11313,7 +11313,7 @@
         <v/>
       </c>
       <c r="E125" t="str">
-        <f t="shared" ref="D125:L188" si="29">MID($B125,E$2,1)</f>
+        <f t="shared" ref="D125:L153" si="29">MID($B125,E$2,1)</f>
         <v/>
       </c>
       <c r="F125" t="str">
@@ -13817,7 +13817,7 @@
         <v/>
       </c>
       <c r="H153" t="str">
-        <f t="shared" ref="D153:L213" si="42">MID($B153,H$2,1)</f>
+        <f t="shared" ref="D153:L181" si="42">MID($B153,H$2,1)</f>
         <v/>
       </c>
       <c r="I153" t="str">
@@ -16321,7 +16321,7 @@
         <v/>
       </c>
       <c r="K181" t="str">
-        <f t="shared" ref="D181:L213" si="43">MID($B181,K$2,1)</f>
+        <f t="shared" ref="D181:L210" si="43">MID($B181,K$2,1)</f>
         <v/>
       </c>
       <c r="L181" t="str">

</xml_diff>